<commit_message>
angular hibernate project day 2
</commit_message>
<xml_diff>
--- a/Project/Advertisement_REST_call_details_v3.xlsx
+++ b/Project/Advertisement_REST_call_details_v3.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -205,7 +205,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,27 +222,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
-      <color rgb="FF00B050"/>
+      <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,7 +237,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -294,34 +286,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,7 +680,7 @@
   <dimension ref="C5:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +784,7 @@
       <c r="F9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="12"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -866,45 +855,45 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="3:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C13" s="4">
+    <row r="13" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13" s="3">
         <v>7</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C14" s="3">
+      <c r="G13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="3:10" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C14" s="12">
         <v>8</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
+      <c r="G14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13" t="s">
         <v>27</v>
       </c>
     </row>
@@ -930,67 +919,67 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="3:10" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C16" s="13">
+    <row r="16" spans="3:10" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="9">
         <v>10</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14" t="s">
+      <c r="G16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="3:12" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C17" s="13">
+    <row r="17" spans="3:12" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C17" s="9">
         <v>11</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14" t="s">
+      <c r="G17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="C18" s="4">
+    <row r="18" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="C18" s="3">
         <v>12</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5" t="s">
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1036,25 +1025,23 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="3">
-        <v>15</v>
-      </c>
-      <c r="D21" s="2" t="s">
+    <row r="21" spans="3:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="4">
+        <v>15</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1084,41 +1071,41 @@
       <c r="C23" s="4">
         <v>17</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12" t="s">
+      <c r="G23" s="5"/>
+      <c r="H23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="3:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="8">
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="3:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="4">
         <v>18</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G24" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="9" t="s">
+      <c r="G24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="5" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>